<commit_message>
New Trend Strategy - Optimize Consolidation
</commit_message>
<xml_diff>
--- a/FundEstimate.xlsx
+++ b/FundEstimate.xlsx
@@ -642,7 +642,7 @@
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>0.33%</t>
+          <t>-0.50%</t>
         </is>
       </c>
       <c r="F3" s="6" t="n">
@@ -654,7 +654,7 @@
       </c>
       <c r="H3" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议高位减持 10.00% 仓位</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="E4" s="6" t="inlineStr">
         <is>
-          <t>0.13%</t>
+          <t>0.76%</t>
         </is>
       </c>
       <c r="F4" s="6" t="n">
@@ -693,7 +693,7 @@
       </c>
       <c r="H4" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
       </c>
       <c r="E5" s="6" t="inlineStr">
         <is>
-          <t>0.73%</t>
+          <t>1.22%</t>
         </is>
       </c>
       <c r="F5" s="6" t="n">
@@ -732,7 +732,7 @@
       </c>
       <c r="H5" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 True，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="E6" s="6" t="inlineStr">
         <is>
-          <t>0.73%</t>
+          <t>1.39%</t>
         </is>
       </c>
       <c r="F6" s="6" t="n">
@@ -771,7 +771,7 @@
       </c>
       <c r="H6" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="E7" s="6" t="inlineStr">
         <is>
-          <t>0.29%</t>
+          <t>-0.50%</t>
         </is>
       </c>
       <c r="F7" s="6" t="n">
@@ -810,7 +810,7 @@
       </c>
       <c r="H7" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议高位减持 10.00% 仓位</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="E8" s="6" t="inlineStr">
         <is>
-          <t>0.72%</t>
+          <t>2.11%</t>
         </is>
       </c>
       <c r="F8" s="6" t="n">
@@ -849,7 +849,7 @@
       </c>
       <c r="H8" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="E9" s="6" t="inlineStr">
         <is>
-          <t>0.63%</t>
+          <t>-0.21%</t>
         </is>
       </c>
       <c r="F9" s="6" t="n">
@@ -888,7 +888,7 @@
       </c>
       <c r="H9" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议低位吸纳 200.00</t>
+          <t>震荡市，未发现操作点：平滑 True，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -915,7 +915,7 @@
       </c>
       <c r="E10" s="6" t="inlineStr">
         <is>
-          <t>0.11%</t>
+          <t>0.71%</t>
         </is>
       </c>
       <c r="F10" s="6" t="n">
@@ -927,7 +927,7 @@
       </c>
       <c r="H10" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -954,7 +954,7 @@
       </c>
       <c r="E11" s="6" t="inlineStr">
         <is>
-          <t>0.28%</t>
+          <t>2.11%</t>
         </is>
       </c>
       <c r="F11" s="6" t="n">
@@ -966,7 +966,7 @@
       </c>
       <c r="H11" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="E12" s="6" t="inlineStr">
         <is>
-          <t>-0.35%</t>
+          <t>2.43%</t>
         </is>
       </c>
       <c r="F12" s="6" t="n">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="H12" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议高位减持 10.00% 仓位</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="E13" s="6" t="inlineStr">
         <is>
-          <t>0.96%</t>
+          <t>0.24%</t>
         </is>
       </c>
       <c r="F13" s="6" t="n">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="H13" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="E14" s="6" t="inlineStr">
         <is>
-          <t>0.29%</t>
+          <t>1.05%</t>
         </is>
       </c>
       <c r="F14" s="6" t="n">
@@ -1083,7 +1083,7 @@
       </c>
       <c r="H14" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="E15" s="6" t="inlineStr">
         <is>
-          <t>0.51%</t>
+          <t>1.52%</t>
         </is>
       </c>
       <c r="F15" s="6" t="n">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="H15" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="E16" s="6" t="inlineStr">
         <is>
-          <t>0.36%</t>
+          <t>1.57%</t>
         </is>
       </c>
       <c r="F16" s="6" t="n">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="H16" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="E17" s="6" t="inlineStr">
         <is>
-          <t>1.71%</t>
+          <t>0.84%</t>
         </is>
       </c>
       <c r="F17" s="6" t="n">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="H17" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="E18" s="6" t="inlineStr">
         <is>
-          <t>-0.18%</t>
+          <t>0.62%</t>
         </is>
       </c>
       <c r="F18" s="6" t="n">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="H18" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="E19" s="6" t="inlineStr">
         <is>
-          <t>0.40%</t>
+          <t>0.54%</t>
         </is>
       </c>
       <c r="F19" s="6" t="n">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="H19" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="E20" s="6" t="inlineStr">
         <is>
-          <t>0.81%</t>
+          <t>0.73%</t>
         </is>
       </c>
       <c r="F20" s="6" t="n">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="H20" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="E21" s="6" t="inlineStr">
         <is>
-          <t>-1.87%</t>
+          <t>-0.70%</t>
         </is>
       </c>
       <c r="F21" s="6" t="n">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="H21" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议高位减持 10.00% 仓位</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="E22" s="6" t="inlineStr">
         <is>
-          <t>-0.03%</t>
+          <t>0.41%</t>
         </is>
       </c>
       <c r="F22" s="6" t="n">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="H22" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议低位吸纳 200.00</t>
+          <t>震荡市，低位吸纳 200.00</t>
         </is>
       </c>
     </row>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="E23" s="6" t="inlineStr">
         <is>
-          <t>0.26%</t>
+          <t>0.78%</t>
         </is>
       </c>
       <c r="F23" s="6" t="n">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="H23" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="E24" s="6" t="inlineStr">
         <is>
-          <t>-0.54%</t>
+          <t>3.16%</t>
         </is>
       </c>
       <c r="F24" s="6" t="n">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="H24" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议高位减持 10.00% 仓位</t>
+          <t>震荡→弱升，试探性建仓 200.00</t>
         </is>
       </c>
     </row>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="E25" s="6" t="inlineStr">
         <is>
-          <t>0.20%</t>
+          <t>-0.40%</t>
         </is>
       </c>
       <c r="F25" s="6" t="n">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="H25" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议高位减持 10.00% 仓位</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="E26" s="6" t="inlineStr">
         <is>
-          <t>-0.09%</t>
+          <t>0.03%</t>
         </is>
       </c>
       <c r="F26" s="6" t="n">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="E27" s="6" t="inlineStr">
         <is>
-          <t>-0.64%</t>
+          <t>2.88%</t>
         </is>
       </c>
       <c r="F27" s="6" t="n">
@@ -1584,7 +1584,7 @@
       </c>
       <c r="H27" s="6" t="inlineStr">
         <is>
-          <t>震荡市，建议高位减持 10.00% 仓位</t>
+          <t>震荡市，未发现操作点：平滑 False，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="E28" s="6" t="inlineStr">
         <is>
-          <t>0.94%</t>
+          <t>0.72%</t>
         </is>
       </c>
       <c r="F28" s="6" t="n">
@@ -1623,7 +1623,7 @@
       </c>
       <c r="H28" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，未发现操作点：平滑 True，成交量无下跌 True，成交量无突破 True</t>
         </is>
       </c>
     </row>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="E29" s="6" t="inlineStr">
         <is>
-          <t>2.69%</t>
+          <t>-0.21%</t>
         </is>
       </c>
       <c r="F29" s="6" t="n">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="H29" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>无操作</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="E30" s="6" t="inlineStr">
         <is>
-          <t>1.34%</t>
+          <t>2.95%</t>
         </is>
       </c>
       <c r="F30" s="6" t="n">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="H30" s="6" t="inlineStr">
         <is>
-          <t>无</t>
+          <t>震荡市，高位减持 -10.00% 仓位</t>
         </is>
       </c>
     </row>

</xml_diff>